<commit_message>
Add: Calculating Sum and Adding Data
</commit_message>
<xml_diff>
--- a/AddfromPy.xlsx
+++ b/AddfromPy.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,24 @@
         <v>65</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4">
+        <f>SUM(B2:B3)/2</f>
+        <v/>
+      </c>
+      <c r="C4">
+        <f>SUM(C2:C3)/2</f>
+        <v/>
+      </c>
+      <c r="D4">
+        <f>SUM(D2:D3)/2</f>
+        <v/>
+      </c>
+      <c r="E4">
+        <f>SUM(E2:E3)/2</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Add: Bold text and Color to cols in Excel
</commit_message>
<xml_diff>
--- a/AddfromPy.xlsx
+++ b/AddfromPy.xlsx
@@ -17,13 +17,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="0099CCFF"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,8 +50,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,27 +427,27 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>NUMBER</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>sub1</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>sub2</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>sub3</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>sub4</t>
         </is>

</xml_diff>